<commit_message>
Managed to print out multiple keyword search results in a neat way and took care of lowercase/uppercase user input. Code is really messy, there's both V1 and V2 functions concurrently, so gotta clean it up
</commit_message>
<xml_diff>
--- a/data_set/canteens.xlsx
+++ b/data_set/canteens.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Project 36 - CZ1003 TA\NTULearn\Assignments\assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/gaox0021_e_ntu_edu_sg/Documents/Y1S2/RE1016 Com Sci/Coding/Food Search/data_set/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_DC747ABCCF13CF768EDCAC5D10400AAA17F503CC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F8D7F771-35A6-974C-9370-34EDE25C54F6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="15060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -284,7 +285,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -345,7 +346,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -623,19 +624,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -652,7 +655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -672,7 +675,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -692,7 +695,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -712,7 +715,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -732,7 +735,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -752,7 +755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -772,7 +775,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -792,7 +795,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -812,7 +815,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -832,7 +835,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -852,7 +855,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -872,7 +875,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -892,7 +895,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -912,7 +915,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -932,7 +935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -952,7 +955,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -972,7 +975,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -992,7 +995,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1072,7 +1075,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1092,7 +1095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1112,7 +1115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1172,7 +1175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>

</xml_diff>